<commit_message>
Updated the task list
</commit_message>
<xml_diff>
--- a/Project_Task_Checklist.xlsx
+++ b/Project_Task_Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iastsoftware20-my.sharepoint.com/personal/sohan_tikare_iast-software_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship Training\Version Control Arkadeep\Assignment\Virtual-Traffic-Light-Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="271" documentId="8_{60CE04EF-DBDF-4BD2-B955-8B69F8F53334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A64EB82-5C04-4A05-B691-C35652ECC892}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F158FDC9-8C79-4B75-A903-88142DBA3754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Title" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Project Title</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Low Level Design (LLD)</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>Detailed design specifications</t>
   </si>
   <si>
@@ -118,12 +115,6 @@
     <t>Module coding and implementation</t>
   </si>
   <si>
-    <t>Prathiksha, Shivaraj &amp; Sohan</t>
-  </si>
-  <si>
-    <t>Nisha &amp; Rakshita</t>
-  </si>
-  <si>
     <t>Test Case Creation</t>
   </si>
   <si>
@@ -133,9 +124,6 @@
     <t>Prathiksha &amp; Nisha</t>
   </si>
   <si>
-    <t>Nireeksha &amp; Keerthana</t>
-  </si>
-  <si>
     <t>Sl.No.</t>
   </si>
   <si>
@@ -188,13 +176,19 @@
   </si>
   <si>
     <t>IASohanT</t>
+  </si>
+  <si>
+    <t>Rakshita, Shivaraj &amp; Sohan</t>
+  </si>
+  <si>
+    <t>Nisha &amp; Nireeksha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,12 +251,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF305496"/>
         <bgColor rgb="FF305496"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -501,13 +489,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -518,33 +506,32 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -854,30 +841,30 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="68.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" customWidth="1"/>
+    <col min="4" max="4" width="68.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" ht="15" thickBot="1"/>
-    <row r="3" spans="3:4" ht="21.95" thickTop="1" thickBot="1">
-      <c r="C3" s="20" t="s">
+    <row r="2" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="3:4" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="22" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="66.95" thickTop="1" thickBot="1">
-      <c r="C4" s="19" t="s">
+    <row r="4" spans="3:4" ht="67" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:4" ht="15" thickTop="1"/>
+    <row r="5" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -888,21 +875,21 @@
   <dimension ref="C6:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" customWidth="1"/>
-    <col min="5" max="5" width="89.7109375" customWidth="1"/>
-    <col min="6" max="6" width="53.42578125" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.453125" customWidth="1"/>
+    <col min="4" max="4" width="33.54296875" customWidth="1"/>
+    <col min="5" max="5" width="89.7265625" customWidth="1"/>
+    <col min="6" max="6" width="53.453125" customWidth="1"/>
+    <col min="7" max="7" width="40.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:7" ht="28.5">
+    <row r="6" spans="3:7" ht="28.5" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
@@ -919,7 +906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="28.5">
+    <row r="7" spans="3:7" ht="28.5" x14ac:dyDescent="0.65">
       <c r="C7" s="9" t="s">
         <v>9</v>
       </c>
@@ -936,12 +923,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="28.5">
+    <row r="8" spans="3:7" ht="28.5" x14ac:dyDescent="0.65">
       <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>15</v>
+      <c r="D8" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>16</v>
@@ -953,55 +940,55 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="28.5">
+    <row r="9" spans="3:7" ht="28.5" x14ac:dyDescent="0.65">
       <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="12" t="s">
+    </row>
+    <row r="10" spans="3:7" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="C10" s="9" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="28.5">
-      <c r="C10" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="C11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="D11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="F11" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="3:7" ht="28.5">
-      <c r="C11" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>31</v>
+      <c r="G11" s="16" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1017,109 +1004,109 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.95" customHeight="1">
-      <c r="A2" s="22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="20">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="20">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.95" customHeight="1">
-      <c r="A3" s="22">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="20">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.95" customHeight="1">
-      <c r="A4" s="22">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="20">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C6" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.95" customHeight="1">
-      <c r="A5" s="22">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C7" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18.95" customHeight="1">
-      <c r="A6" s="22">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="20">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18.95" customHeight="1">
-      <c r="A7" s="22">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
+    <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="21">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.95" customHeight="1">
-      <c r="A8" s="22">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.95" customHeight="1">
-      <c r="A9" s="23">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project task Checklist updated
</commit_message>
<xml_diff>
--- a/Project_Task_Checklist.xlsx
+++ b/Project_Task_Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship Training\Version Control Arkadeep\Assignment\Virtual-Traffic-Light-Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iastsoftware20-my.sharepoint.com/personal/prathiksha_jain_iast-software_com/Documents/Desktop/Virtual-Traffic-Light-Controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F158FDC9-8C79-4B75-A903-88142DBA3754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{F158FDC9-8C79-4B75-A903-88142DBA3754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F888D36-5F5A-4F0D-A649-84B0A2615203}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="2790" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Title" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Project Title</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>High Level Design (HLD)</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>System architecture and component breakdown</t>
@@ -240,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,12 +253,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,13 +480,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -509,29 +500,28 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -849,18 +839,18 @@
   <sheetData>
     <row r="2" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="3:4" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="67" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -874,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C6:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -931,63 +921,63 @@
         <v>10</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="3:7" ht="28.5" x14ac:dyDescent="0.65">
       <c r="C9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="12" t="s">
         <v>21</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="3:7" ht="28.5" x14ac:dyDescent="0.65">
       <c r="C10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="C11" s="14" t="s">
+      <c r="D11" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1012,101 +1002,101 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="2" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="23" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="23" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="19">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="23" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="23" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="19">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="23" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="20">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="23" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="21">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="23" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>